<commit_message>
Lengths from UVC transformed from TL to FL before doing KDE, to enable comparison between UVC and stereo-DOVs.
</commit_message>
<xml_diff>
--- a/Data/LengthRatio.xlsx
+++ b/Data/LengthRatio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ejer\Desktop\Github_UVC_DOVS\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CCB0BC92-F7CB-4CF8-94EA-EA39D342540D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0596F51C-BC44-47C6-9CA5-5B3540AF4AE3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00DD2FDA-E2AD-4D59-AD14-348934C399C8}"/>
   </bookViews>
@@ -95,7 +95,7 @@
     <t>Aetobatus laticeps</t>
   </si>
   <si>
-    <t>Caranx lugubris</t>
+    <t>Caranx lugubris</t>
   </si>
 </sst>
 </file>
@@ -462,7 +462,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>